<commit_message>
chore: update filtered_output.xlsx via GitHub Actions
</commit_message>
<xml_diff>
--- a/data/filtered_output.xlsx
+++ b/data/filtered_output.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,231 +484,297 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EICHERMOT</t>
+          <t>INDUSINDBK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5684.5</v>
+        <v>801.85</v>
       </c>
       <c r="C2" t="n">
-        <v>5712.5</v>
+        <v>810</v>
       </c>
       <c r="D2" t="n">
-        <v>5651</v>
+        <v>789.1</v>
       </c>
       <c r="E2" t="n">
-        <v>5665.5</v>
+        <v>808.6</v>
       </c>
       <c r="F2" t="n">
-        <v>202535</v>
+        <v>2553303</v>
       </c>
       <c r="G2" t="n">
-        <v>458305</v>
+        <v>5249912</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.5580781357393002</v>
+        <v>-0.5136484192496941</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>EICHERMOT</t>
+          <t>INDUSINDBK</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GRASIM</t>
+          <t>INDIGO</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2800</v>
+        <v>5893.5</v>
       </c>
       <c r="C3" t="n">
-        <v>2800</v>
+        <v>5907</v>
       </c>
       <c r="D3" t="n">
-        <v>2758</v>
+        <v>5793.5</v>
       </c>
       <c r="E3" t="n">
-        <v>2764</v>
+        <v>5884</v>
       </c>
       <c r="F3" t="n">
-        <v>393906</v>
+        <v>483125</v>
       </c>
       <c r="G3" t="n">
-        <v>782631</v>
+        <v>980678</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.4966900110013531</v>
+        <v>-0.507356135245208</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>GRASIM</t>
+          <t>INDIGO</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SIEMENS</t>
+          <t>BSE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3100</v>
+        <v>2370</v>
       </c>
       <c r="C4" t="n">
-        <v>3114</v>
+        <v>2454</v>
       </c>
       <c r="D4" t="n">
-        <v>3057</v>
+        <v>2359.3</v>
       </c>
       <c r="E4" t="n">
-        <v>3083</v>
+        <v>2452</v>
       </c>
       <c r="F4" t="n">
-        <v>392854</v>
+        <v>4564283</v>
       </c>
       <c r="G4" t="n">
-        <v>772626</v>
+        <v>9401319</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.4915340669353607</v>
+        <v>-0.5145061028138711</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>SIEMENS</t>
+          <t>BSE</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NAUKRI</t>
+          <t>POLYCAB</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1341.7</v>
+        <v>6790</v>
       </c>
       <c r="C5" t="n">
-        <v>1345</v>
+        <v>6903.5</v>
       </c>
       <c r="D5" t="n">
-        <v>1311.5</v>
+        <v>6746</v>
       </c>
       <c r="E5" t="n">
-        <v>1321</v>
+        <v>6896</v>
       </c>
       <c r="F5" t="n">
-        <v>1704636</v>
+        <v>193378</v>
       </c>
       <c r="G5" t="n">
-        <v>3593587</v>
+        <v>444662</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.5256449892544691</v>
+        <v>-0.565112377491218</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>NAUKRI</t>
+          <t>POLYCAB</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DABUR</t>
+          <t>SBICARD</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>524.15</v>
+        <v>787.3</v>
       </c>
       <c r="C6" t="n">
-        <v>524.15</v>
+        <v>799</v>
       </c>
       <c r="D6" t="n">
-        <v>512</v>
+        <v>784</v>
       </c>
       <c r="E6" t="n">
-        <v>514</v>
+        <v>799</v>
       </c>
       <c r="F6" t="n">
-        <v>931299</v>
+        <v>526708</v>
       </c>
       <c r="G6" t="n">
-        <v>2027038</v>
+        <v>1239184</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.5405616470929504</v>
+        <v>-0.5749557773502563</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>DABUR</t>
+          <t>SBICARD</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ASTRAL</t>
+          <t>MARICO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1430</v>
+        <v>712.15</v>
       </c>
       <c r="C7" t="n">
-        <v>1430.6</v>
+        <v>719.9</v>
       </c>
       <c r="D7" t="n">
-        <v>1403</v>
+        <v>707.25</v>
       </c>
       <c r="E7" t="n">
-        <v>1418</v>
+        <v>718.1</v>
       </c>
       <c r="F7" t="n">
-        <v>211740</v>
+        <v>977299</v>
       </c>
       <c r="G7" t="n">
-        <v>451543</v>
+        <v>2396780</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.5310745598979499</v>
+        <v>-0.5922450120578443</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>ASTRAL</t>
+          <t>MARICO</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NUVAMA</t>
+          <t>AMBER</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7000</v>
+        <v>7595</v>
       </c>
       <c r="C8" t="n">
-        <v>7025</v>
+        <v>7785</v>
       </c>
       <c r="D8" t="n">
-        <v>6850</v>
+        <v>7595</v>
       </c>
       <c r="E8" t="n">
-        <v>6992</v>
+        <v>7765</v>
       </c>
       <c r="F8" t="n">
-        <v>100383</v>
+        <v>185434</v>
       </c>
       <c r="G8" t="n">
-        <v>200401</v>
+        <v>397729</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.4990893259015673</v>
+        <v>-0.5337679676362549</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>NUVAMA</t>
+          <t>AMBER</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ANGELONE</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2576</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2653</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2576</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2645.8</v>
+      </c>
+      <c r="F9" t="n">
+        <v>543383</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1180598</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-0.5397391830241962</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>ANGELONE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>IIFL</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>452</v>
+      </c>
+      <c r="C10" t="n">
+        <v>455.4</v>
+      </c>
+      <c r="D10" t="n">
+        <v>441.1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>453.35</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1488749</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3539104</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-0.5793429636427752</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>IIFL</t>
         </is>
       </c>
     </row>
@@ -723,7 +789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,66 +847,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NTPC</t>
+          <t>TECHM</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>333.6</v>
+        <v>1455</v>
       </c>
       <c r="C2" t="n">
-        <v>335.4</v>
+        <v>1492</v>
       </c>
       <c r="D2" t="n">
-        <v>331.6</v>
+        <v>1450</v>
       </c>
       <c r="E2" t="n">
-        <v>332.55</v>
+        <v>1488.1</v>
       </c>
       <c r="F2" t="n">
-        <v>13872826</v>
+        <v>1587489</v>
       </c>
       <c r="G2" t="n">
-        <v>9855535</v>
+        <v>1039973</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4076177498228153</v>
+        <v>0.526471360314162</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>NTPC</t>
+          <t>TECHM</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ETERNAL</t>
+          <t>BAJFINANCE</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>302</v>
+        <v>871</v>
       </c>
       <c r="C3" t="n">
-        <v>302.5</v>
+        <v>882</v>
       </c>
       <c r="D3" t="n">
-        <v>295.45</v>
+        <v>867.25</v>
       </c>
       <c r="E3" t="n">
-        <v>300.05</v>
+        <v>881.9</v>
       </c>
       <c r="F3" t="n">
-        <v>22012280</v>
+        <v>5998002</v>
       </c>
       <c r="G3" t="n">
-        <v>14820256</v>
+        <v>4212648</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4852833851183138</v>
+        <v>0.4238080181396594</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ETERNAL</t>
+          <t>BAJFINANCE</t>
         </is>
       </c>
     </row>
@@ -851,25 +917,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1629.7</v>
+        <v>1581</v>
       </c>
       <c r="C4" t="n">
-        <v>1629.7</v>
+        <v>1605.4</v>
       </c>
       <c r="D4" t="n">
-        <v>1591</v>
+        <v>1571</v>
       </c>
       <c r="E4" t="n">
-        <v>1593.5</v>
+        <v>1599.5</v>
       </c>
       <c r="F4" t="n">
+        <v>3435674</v>
+      </c>
+      <c r="G4" t="n">
         <v>2376257</v>
       </c>
-      <c r="G4" t="n">
-        <v>1622897</v>
-      </c>
       <c r="H4" t="n">
-        <v>0.4642069090028511</v>
+        <v>0.4458343520923873</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -880,330 +946,396 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PIDILITIND</t>
+          <t>JIOFIN</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3026</v>
+        <v>323</v>
       </c>
       <c r="C5" t="n">
-        <v>3058</v>
+        <v>328</v>
       </c>
       <c r="D5" t="n">
-        <v>2973.1</v>
+        <v>316.8</v>
       </c>
       <c r="E5" t="n">
-        <v>3042</v>
+        <v>327.4</v>
       </c>
       <c r="F5" t="n">
-        <v>819116</v>
+        <v>16461908</v>
       </c>
       <c r="G5" t="n">
-        <v>577583</v>
+        <v>11615135</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4181788591423224</v>
+        <v>0.4172808150744696</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>PIDILITIND</t>
+          <t>JIOFIN</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>LICI</t>
+          <t>GRASIM</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>890</v>
+        <v>2764</v>
       </c>
       <c r="C6" t="n">
-        <v>902</v>
+        <v>2772.7</v>
       </c>
       <c r="D6" t="n">
-        <v>888</v>
+        <v>2718.8</v>
       </c>
       <c r="E6" t="n">
-        <v>895</v>
+        <v>2741.9</v>
       </c>
       <c r="F6" t="n">
-        <v>691080</v>
+        <v>591589</v>
       </c>
       <c r="G6" t="n">
-        <v>454682</v>
+        <v>393906</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5199194162073713</v>
+        <v>0.5018532340202992</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>LICI</t>
+          <t>GRASIM</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INDHOTEL</t>
+          <t>TORNTPHARM</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>751.05</v>
+        <v>3490.2</v>
       </c>
       <c r="C7" t="n">
-        <v>755.45</v>
+        <v>3637</v>
       </c>
       <c r="D7" t="n">
-        <v>739.5</v>
+        <v>3490.2</v>
       </c>
       <c r="E7" t="n">
-        <v>743.05</v>
+        <v>3595</v>
       </c>
       <c r="F7" t="n">
-        <v>2431229</v>
+        <v>402653</v>
       </c>
       <c r="G7" t="n">
-        <v>1553257</v>
+        <v>257376</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5652458028516852</v>
+        <v>0.564454339176924</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>INDHOTEL</t>
+          <t>TORNTPHARM</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>VBL</t>
+          <t>PIDILITIND</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>506</v>
+        <v>3057</v>
       </c>
       <c r="C8" t="n">
-        <v>507.95</v>
+        <v>3117.9</v>
       </c>
       <c r="D8" t="n">
-        <v>497.25</v>
+        <v>3022.8</v>
       </c>
       <c r="E8" t="n">
-        <v>498.05</v>
+        <v>3051</v>
       </c>
       <c r="F8" t="n">
-        <v>3191536</v>
+        <v>1176910</v>
       </c>
       <c r="G8" t="n">
-        <v>2223010</v>
+        <v>819116</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4356822506421474</v>
+        <v>0.4368050434859043</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>VBL</t>
+          <t>PIDILITIND</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CUMMINSIND</t>
+          <t>IRFC</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3638</v>
+        <v>127</v>
       </c>
       <c r="C9" t="n">
-        <v>3672.6</v>
+        <v>127.95</v>
       </c>
       <c r="D9" t="n">
-        <v>3599.8</v>
+        <v>124.1</v>
       </c>
       <c r="E9" t="n">
-        <v>3629.8</v>
+        <v>127.9</v>
       </c>
       <c r="F9" t="n">
-        <v>899245</v>
+        <v>9602587</v>
       </c>
       <c r="G9" t="n">
-        <v>634486</v>
+        <v>6331289</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4172810747597268</v>
+        <v>0.5166875181341429</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>CUMMINSIND</t>
+          <t>IRFC</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HINDZINC</t>
+          <t>LUPIN</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>422.7</v>
+        <v>1855.9</v>
       </c>
       <c r="C10" t="n">
-        <v>423.9</v>
+        <v>1952.7</v>
       </c>
       <c r="D10" t="n">
-        <v>416.85</v>
+        <v>1855</v>
       </c>
       <c r="E10" t="n">
-        <v>419.8</v>
+        <v>1937.3</v>
       </c>
       <c r="F10" t="n">
-        <v>1418372</v>
+        <v>4166570</v>
       </c>
       <c r="G10" t="n">
-        <v>990246</v>
+        <v>2735877</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4323430743471824</v>
+        <v>0.5229376174440591</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>HINDZINC</t>
+          <t>LUPIN</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KPITTECH</t>
+          <t>POLICYBZR</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1204.3</v>
+        <v>1730</v>
       </c>
       <c r="C11" t="n">
-        <v>1214.1</v>
+        <v>1790</v>
       </c>
       <c r="D11" t="n">
-        <v>1195.1</v>
+        <v>1725</v>
       </c>
       <c r="E11" t="n">
-        <v>1205</v>
+        <v>1786.3</v>
       </c>
       <c r="F11" t="n">
-        <v>486218</v>
+        <v>1072869</v>
       </c>
       <c r="G11" t="n">
-        <v>336953</v>
+        <v>710140</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4429846299038738</v>
+        <v>0.5107851972850423</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>KPITTECH</t>
+          <t>POLICYBZR</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BANDHANBNK</t>
+          <t>IREDA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>166.75</v>
+        <v>143.8</v>
       </c>
       <c r="C12" t="n">
-        <v>166.8</v>
+        <v>145.45</v>
       </c>
       <c r="D12" t="n">
-        <v>163.91</v>
+        <v>140.26</v>
       </c>
       <c r="E12" t="n">
-        <v>164.45</v>
+        <v>145.45</v>
       </c>
       <c r="F12" t="n">
-        <v>4382033</v>
+        <v>6734089</v>
       </c>
       <c r="G12" t="n">
-        <v>3028618</v>
+        <v>4802241</v>
       </c>
       <c r="H12" t="n">
-        <v>0.44687543955692</v>
+        <v>0.4022805186162044</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>BANDHANBNK</t>
+          <t>IREDA</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NYKAA</t>
+          <t>ATGL</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>211.39</v>
+        <v>589</v>
       </c>
       <c r="C13" t="n">
-        <v>212.54</v>
+        <v>594.75</v>
       </c>
       <c r="D13" t="n">
-        <v>207.15</v>
+        <v>577.1</v>
       </c>
       <c r="E13" t="n">
-        <v>207.9</v>
+        <v>591</v>
       </c>
       <c r="F13" t="n">
-        <v>2875309</v>
+        <v>631605</v>
       </c>
       <c r="G13" t="n">
-        <v>1895822</v>
+        <v>404411</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5166555720948486</v>
+        <v>0.5617898622935578</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>NYKAA</t>
+          <t>ATGL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>JUBLFOOD</t>
+          <t>SUZLON</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>643.9</v>
+        <v>64.81</v>
       </c>
       <c r="C14" t="n">
-        <v>643.9</v>
+        <v>65.26000000000001</v>
       </c>
       <c r="D14" t="n">
-        <v>625.35</v>
+        <v>62.21</v>
       </c>
       <c r="E14" t="n">
-        <v>629.95</v>
+        <v>64.2</v>
       </c>
       <c r="F14" t="n">
-        <v>1035230</v>
+        <v>75542321</v>
       </c>
       <c r="G14" t="n">
-        <v>707823</v>
+        <v>47280146</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4625549042627888</v>
+        <v>0.597759892704223</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>JUBLFOOD</t>
+          <t>SUZLON</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SRF</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2965</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2965</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2875</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2913</v>
+      </c>
+      <c r="F15" t="n">
+        <v>479056</v>
+      </c>
+      <c r="G15" t="n">
+        <v>321329</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.4908582792091595</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>SRF</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MANAPPURAM</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>255.6</v>
+      </c>
+      <c r="C16" t="n">
+        <v>263.15</v>
+      </c>
+      <c r="D16" t="n">
+        <v>253.7</v>
+      </c>
+      <c r="E16" t="n">
+        <v>261.9</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2066794</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1423890</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.4515124061549698</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>MANAPPURAM</t>
         </is>
       </c>
     </row>

</xml_diff>